<commit_message>
Update shift scheduling constraints and add availability checking functionality
</commit_message>
<xml_diff>
--- a/shift_schedule.xlsx
+++ b/shift_schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="57">
   <si>
     <t>Day</t>
   </si>
@@ -31,13 +31,13 @@
     <t>2:00AM - 8:00AM</t>
   </si>
   <si>
-    <t>Gabe Heller (7187220895) (D), Paul (3106583636) (D)</t>
+    <t>Jack Mogelof (9172163044) (D), Alejandro L (2676633214)</t>
   </si>
   <si>
     <t>8:00AM - 11:00AM</t>
   </si>
   <si>
-    <t>Alexander (9175433831) (D), Jamari Pitchford (7738297627) (D), Jake Dieterich (9177968225)</t>
+    <t>Josh Greene (9176368454) (D), Thor Waguespack (2404299065) (D), Ali Awada (6469771844)</t>
   </si>
   <si>
     <t>11:00AM - 2:00PM</t>
@@ -49,55 +49,55 @@
     <t>2:00PM - 5:00PM</t>
   </si>
   <si>
-    <t>Jaxon (4159881691) (D), Henry (6073399363), Blake Steel (6109995081) (D)</t>
+    <t>Jaxon (4159881691) (D), Jake Dieterich (9177968225), Blake Steel (6109995081) (D)</t>
   </si>
   <si>
     <t>5:00PM - 8:00PM</t>
   </si>
   <si>
-    <t>Ben Kairouz (9179401653) (D), Alejandro Espinosa (7866702380) (D), Harry Corbin (5182223247) (D)</t>
+    <t>Alexander (9175433831) (D), Henry (6073399363), Harry Corbin (5182223247) (D)</t>
   </si>
   <si>
     <t>8:00PM - 11:00PM</t>
   </si>
   <si>
-    <t>Jack Mogelof (9172163044) (D), Alejandro L (2676633214), Noah Yaffe (6109995081) (D)</t>
+    <t>Alejandro Espinosa (7866702380) (D), Jamari Pitchford (7738297627) (D), Adi (3103038889) (D)</t>
   </si>
   <si>
     <t>11:00PM - 2:00AM</t>
   </si>
   <si>
-    <t>Josh Greene (9176368454) (D), Thor Waguespack (2404299065) (D), Ali Awada (6469771844)</t>
+    <t>George Ryckman (9176015863) (D), Alejandro E. Ulvert (3058421968) (D), Noah Yaffe (6109995081) (D)</t>
   </si>
   <si>
     <t>Tuesday</t>
   </si>
   <si>
-    <t>Josh Greene (9176368454) (D), Alejandro L (2676633214)</t>
-  </si>
-  <si>
-    <t>Paul (3106583636) (D), Jamari Pitchford (7738297627) (D), Thor Waguespack (2404299065) (D)</t>
-  </si>
-  <si>
-    <t>Jack Mogelof (9172163044) (D), Blake Steel (6109995081) (D)</t>
-  </si>
-  <si>
-    <t>Ben Kairouz (9179401653) (D), Kamsi (6465933923), George Ryckman (9176015863) (D)</t>
-  </si>
-  <si>
-    <t>Ezana (2405594003), Alexander (9175433831) (D), Alejandro Espinosa (7866702380) (D)</t>
-  </si>
-  <si>
-    <t>Henry (6073399363), Matheo (6462079196) (D), Noah Yaffe (6109995081) (D)</t>
+    <t>Alexander (9175433831) (D), Henry (6073399363)</t>
+  </si>
+  <si>
+    <t>Thor Waguespack (2404299065) (D), Edu (7862012521) (D), Adi (3103038889) (D)</t>
+  </si>
+  <si>
+    <t>Jack Mogelof (9172163044) (D), Ben Kairouz (9179401653) (D)</t>
+  </si>
+  <si>
+    <t>Ezana (2405594003), George Ryckman (9176015863) (D)</t>
+  </si>
+  <si>
+    <t>Jake Dieterich (9177968225), Alejandro E. Ulvert (3058421968) (D), Noah Yaffe (6109995081) (D)</t>
+  </si>
+  <si>
+    <t>Jaxon (4159881691) (D), Paul (3106583636) (D), Alejandro Espinosa (7866702380) (D)</t>
   </si>
   <si>
     <t>Wednesday</t>
   </si>
   <si>
-    <t>Jamari Pitchford (7738297627) (D), Jake Dieterich (9177968225)</t>
-  </si>
-  <si>
-    <t>Gabe Heller (7187220895) (D), Paul (3106583636) (D), Thor Waguespack (2404299065) (D)</t>
+    <t>Jake Dieterich (9177968225), Adi (3103038889) (D)</t>
+  </si>
+  <si>
+    <t>Paul (3106583636) (D), Josh Greene (9176368454) (D), Ali Awada (6469771844)</t>
   </si>
   <si>
     <t>Jaxon (4159881691) (D), Matheo (6462079196) (D), Blake Steel (6109995081) (D)</t>
@@ -106,22 +106,25 @@
     <t>Henry (6073399363), Edu (7862012521) (D)</t>
   </si>
   <si>
-    <t>Ezana (2405594003), Josh Greene (9176368454) (D), Adi (3103038889) (D)</t>
-  </si>
-  <si>
-    <t>Alejandro L (2676633214), Alejandro E. Ulvert (3058421968) (D), Noah Yaffe (6109995081) (D)</t>
-  </si>
-  <si>
-    <t>Ben Kairouz (9179401653) (D), Kamsi (6465933923), Alexander (9175433831) (D)</t>
+    <t>Ezana (2405594003), Jamari Pitchford (7738297627) (D), Harry Corbin (5182223247) (D)</t>
+  </si>
+  <si>
+    <t>Kamsi (6465933923), Alejandro Espinosa (7866702380) (D), Noah Yaffe (6109995081) (D)</t>
+  </si>
+  <si>
+    <t>Gabe Heller (7187220895) (D), Alexander (9175433831) (D), Alejandro L (2676633214)</t>
   </si>
   <si>
     <t>Thursday</t>
   </si>
   <si>
-    <t>Ali Awada (6469771844), Adi (3103038889) (D)</t>
-  </si>
-  <si>
-    <t>Paul (3106583636) (D), Josh Greene (9176368454) (D), Edu (7862012521) (D)</t>
+    <t>Ezana (2405594003), Matheo (6462079196) (D)</t>
+  </si>
+  <si>
+    <t>Paul (3106583636) (D), Thor Waguespack (2404299065) (D), Edu (7862012521) (D)</t>
+  </si>
+  <si>
+    <t>Jack Mogelof (9172163044) (D)</t>
   </si>
   <si>
     <t>Ben Kairouz (9179401653) (D), Kamsi (6465933923)</t>
@@ -130,58 +133,58 @@
     <t>Friday</t>
   </si>
   <si>
-    <t>Ezana (2405594003), Harry Corbin (5182223247) (D)</t>
-  </si>
-  <si>
-    <t>Kamsi (6465933923), Matheo (6462079196) (D), Alejandro Espinosa (7866702380) (D)</t>
-  </si>
-  <si>
-    <t>Jamari Pitchford (7738297627) (D), Edu (7862012521) (D), Blake Steel (6109995081) (D)</t>
+    <t>Gabe Heller (7187220895) (D), Kamsi (6465933923)</t>
+  </si>
+  <si>
+    <t>Jaxon (4159881691) (D), Paul (3106583636) (D), Alejandro L (2676633214)</t>
+  </si>
+  <si>
+    <t>Jack Mogelof (9172163044) (D), Jamari Pitchford (7738297627) (D), Edu (7862012521) (D)</t>
   </si>
   <si>
     <t>Ben Kairouz (9179401653) (D), Thor Waguespack (2404299065) (D), Alejandro E. Ulvert (3058421968) (D)</t>
   </si>
   <si>
-    <t>Gabe Heller (7187220895) (D), Paul (3106583636) (D), Ali Awada (6469771844)</t>
+    <t>Ali Awada (6469771844), Blake Steel (6109995081) (D), Harry Corbin (5182223247) (D)</t>
   </si>
   <si>
     <t>Saturday</t>
   </si>
   <si>
-    <t>Jack Mogelof (9172163044) (D), Alejandro E. Ulvert (3058421968) (D)</t>
-  </si>
-  <si>
-    <t>Kamsi (6465933923), Alejandro Espinosa (7866702380) (D), Adi (3103038889) (D)</t>
-  </si>
-  <si>
-    <t>Gabe Heller (7187220895) (D), Alejandro L (2676633214), Harry Corbin (5182223247) (D)</t>
-  </si>
-  <si>
-    <t>Jaxon (4159881691) (D), Ben Kairouz (9179401653) (D), Henry (6073399363)</t>
-  </si>
-  <si>
-    <t>Alexander (9175433831) (D), Edu (7862012521) (D), George Ryckman (9176015863) (D)</t>
+    <t>Gabe Heller (7187220895) (D), Harry Corbin (5182223247) (D)</t>
+  </si>
+  <si>
+    <t>Jaxon (4159881691) (D), Alejandro L (2676633214), Alejandro Espinosa (7866702380) (D)</t>
+  </si>
+  <si>
+    <t>Josh Greene (9176368454) (D), Ali Awada (6469771844), Alejandro E. Ulvert (3058421968) (D)</t>
+  </si>
+  <si>
+    <t>Ben Kairouz (9179401653) (D), Paul (3106583636) (D), George Ryckman (9176015863) (D)</t>
+  </si>
+  <si>
+    <t>Jamari Pitchford (7738297627) (D), Jake Dieterich (9177968225), Blake Steel (6109995081) (D)</t>
   </si>
   <si>
     <t>Sunday</t>
   </si>
   <si>
-    <t>Jaxon (4159881691) (D), George Ryckman (9176015863) (D)</t>
-  </si>
-  <si>
-    <t>Josh Greene (9176368454) (D), Alejandro L (2676633214), Harry Corbin (5182223247) (D)</t>
-  </si>
-  <si>
-    <t>Matheo (6462079196) (D), Jake Dieterich (9177968225), Adi (3103038889) (D)</t>
-  </si>
-  <si>
-    <t>Gabe Heller (7187220895) (D), Ezana (2405594003), Alejandro Espinosa (7866702380) (D)</t>
-  </si>
-  <si>
-    <t>Henry (6073399363), Alejandro E. Ulvert (3058421968) (D), Noah Yaffe (6109995081) (D)</t>
-  </si>
-  <si>
-    <t>Jack Mogelof (9172163044) (D), Kamsi (6465933923), Blake Steel (6109995081) (D)</t>
+    <t>Josh Greene (9176368454) (D), George Ryckman (9176015863) (D)</t>
+  </si>
+  <si>
+    <t>Kamsi (6465933923), Alexander (9175433831) (D), Alejandro Espinosa (7866702380) (D)</t>
+  </si>
+  <si>
+    <t>Matheo (6462079196) (D), Edu (7862012521) (D), Ali Awada (6469771844)</t>
+  </si>
+  <si>
+    <t>Ben Kairouz (9179401653) (D), Henry (6073399363), Thor Waguespack (2404299065) (D)</t>
+  </si>
+  <si>
+    <t>Jamari Pitchford (7738297627) (D), Blake Steel (6109995081) (D), Noah Yaffe (6109995081) (D)</t>
+  </si>
+  <si>
+    <t>Ezana (2405594003), Alejandro E. Ulvert (3058421968) (D), Adi (3103038889) (D)</t>
   </si>
 </sst>
 </file>
@@ -780,7 +783,7 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -791,183 +794,183 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
         <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
         <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B37" t="s">
         <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B41" t="s">
         <v>16</v>
       </c>
       <c r="C41" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update availability check example and modify processed student availability data
</commit_message>
<xml_diff>
--- a/shift_schedule.xlsx
+++ b/shift_schedule.xlsx
@@ -31,13 +31,13 @@
     <t>2:00AM - 8:00AM</t>
   </si>
   <si>
-    <t>Jack Mogelof (9172163044) (D), Alejandro L (2676633214)</t>
+    <t>Alejandro E. Ulvert (3058421968) (D), Adi (3103038889) (D)</t>
   </si>
   <si>
     <t>8:00AM - 11:00AM</t>
   </si>
   <si>
-    <t>Josh Greene (9176368454) (D), Thor Waguespack (2404299065) (D), Ali Awada (6469771844)</t>
+    <t>Alexander (9175433831) (D), Alejandro L (2676633214), Thor Waguespack (2404299065) (D)</t>
   </si>
   <si>
     <t>11:00AM - 2:00PM</t>
@@ -55,136 +55,136 @@
     <t>5:00PM - 8:00PM</t>
   </si>
   <si>
-    <t>Alexander (9175433831) (D), Henry (6073399363), Harry Corbin (5182223247) (D)</t>
+    <t>Kamsi (6465933923), Alejandro Espinosa (7866702380) (D), Harry Corbin (5182223247) (D)</t>
   </si>
   <si>
     <t>8:00PM - 11:00PM</t>
   </si>
   <si>
-    <t>Alejandro Espinosa (7866702380) (D), Jamari Pitchford (7738297627) (D), Adi (3103038889) (D)</t>
+    <t>Ezana (2405594003), Paul (3106583636) (D), George Ryckman (9176015863) (D)</t>
   </si>
   <si>
     <t>11:00PM - 2:00AM</t>
   </si>
   <si>
-    <t>George Ryckman (9176015863) (D), Alejandro E. Ulvert (3058421968) (D), Noah Yaffe (6109995081) (D)</t>
+    <t>Jamari Pitchford (7738297627) (D), Edu (7862012521) (D), Noah Yaffe (6109995081) (D)</t>
   </si>
   <si>
     <t>Tuesday</t>
   </si>
   <si>
-    <t>Alexander (9175433831) (D), Henry (6073399363)</t>
-  </si>
-  <si>
-    <t>Thor Waguespack (2404299065) (D), Edu (7862012521) (D), Adi (3103038889) (D)</t>
+    <t>Adi (3103038889) (D), Harry Corbin (5182223247) (D)</t>
+  </si>
+  <si>
+    <t>Paul (3106583636) (D), Josh Greene (9176368454) (D), Alejandro E. Ulvert (3058421968) (D)</t>
   </si>
   <si>
     <t>Jack Mogelof (9172163044) (D), Ben Kairouz (9179401653) (D)</t>
   </si>
   <si>
-    <t>Ezana (2405594003), George Ryckman (9176015863) (D)</t>
-  </si>
-  <si>
-    <t>Jake Dieterich (9177968225), Alejandro E. Ulvert (3058421968) (D), Noah Yaffe (6109995081) (D)</t>
-  </si>
-  <si>
-    <t>Jaxon (4159881691) (D), Paul (3106583636) (D), Alejandro Espinosa (7866702380) (D)</t>
+    <t>Ali Awada (6469771844), George Ryckman (9176015863) (D)</t>
+  </si>
+  <si>
+    <t>Alejandro Espinosa (7866702380) (D), Edu (7862012521) (D), Blake Steel (6109995081) (D)</t>
+  </si>
+  <si>
+    <t>Matheo (6462079196) (D), Jake Dieterich (9177968225), Noah Yaffe (6109995081) (D)</t>
   </si>
   <si>
     <t>Wednesday</t>
   </si>
   <si>
-    <t>Jake Dieterich (9177968225), Adi (3103038889) (D)</t>
-  </si>
-  <si>
-    <t>Paul (3106583636) (D), Josh Greene (9176368454) (D), Ali Awada (6469771844)</t>
-  </si>
-  <si>
-    <t>Jaxon (4159881691) (D), Matheo (6462079196) (D), Blake Steel (6109995081) (D)</t>
-  </si>
-  <si>
-    <t>Henry (6073399363), Edu (7862012521) (D)</t>
-  </si>
-  <si>
-    <t>Ezana (2405594003), Jamari Pitchford (7738297627) (D), Harry Corbin (5182223247) (D)</t>
-  </si>
-  <si>
-    <t>Kamsi (6465933923), Alejandro Espinosa (7866702380) (D), Noah Yaffe (6109995081) (D)</t>
-  </si>
-  <si>
-    <t>Gabe Heller (7187220895) (D), Alexander (9175433831) (D), Alejandro L (2676633214)</t>
+    <t>George Ryckman (9176015863) (D), Jake Dieterich (9177968225)</t>
+  </si>
+  <si>
+    <t>Alejandro L (2676633214), Alejandro Espinosa (7866702380) (D), Thor Waguespack (2404299065) (D)</t>
+  </si>
+  <si>
+    <t>Jaxon (4159881691) (D), Matheo (6462079196) (D)</t>
+  </si>
+  <si>
+    <t>Henry (6073399363), Edu (7862012521) (D), Blake Steel (6109995081) (D)</t>
+  </si>
+  <si>
+    <t>Gabe Heller (7187220895) (D), Kamsi (6465933923), Josh Greene (9176368454) (D)</t>
+  </si>
+  <si>
+    <t>Ben Kairouz (9179401653) (D), Alexander (9175433831) (D), Alejandro E. Ulvert (3058421968) (D)</t>
+  </si>
+  <si>
+    <t>Ezana (2405594003), Jamari Pitchford (7738297627) (D), Noah Yaffe (6109995081) (D)</t>
   </si>
   <si>
     <t>Thursday</t>
   </si>
   <si>
+    <t>Kamsi (6465933923), Blake Steel (6109995081) (D)</t>
+  </si>
+  <si>
+    <t>Gabe Heller (7187220895) (D), Josh Greene (9176368454) (D), Thor Waguespack (2404299065) (D)</t>
+  </si>
+  <si>
+    <t>Jack Mogelof (9172163044) (D)</t>
+  </si>
+  <si>
+    <t>Ben Kairouz (9179401653) (D), Ali Awada (6469771844)</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Henry (6073399363), Thor Waguespack (2404299065) (D)</t>
+  </si>
+  <si>
+    <t>Jaxon (4159881691) (D), Gabe Heller (7187220895) (D), Alejandro Espinosa (7866702380) (D)</t>
+  </si>
+  <si>
+    <t>Jack Mogelof (9172163044) (D), Jamari Pitchford (7738297627) (D), Edu (7862012521) (D)</t>
+  </si>
+  <si>
+    <t>Ben Kairouz (9179401653) (D), Alejandro E. Ulvert (3058421968) (D), Harry Corbin (5182223247) (D)</t>
+  </si>
+  <si>
+    <t>Paul (3106583636) (D), Alexander (9175433831) (D), Alejandro L (2676633214)</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Jamari Pitchford (7738297627) (D), Ali Awada (6469771844)</t>
+  </si>
+  <si>
+    <t>Jack Mogelof (9172163044) (D), Alejandro L (2676633214), George Ryckman (9176015863) (D)</t>
+  </si>
+  <si>
+    <t>Gabe Heller (7187220895) (D), Alexander (9175433831) (D), Edu (7862012521) (D)</t>
+  </si>
+  <si>
+    <t>Jaxon (4159881691) (D), Ezana (2405594003), Josh Greene (9176368454) (D)</t>
+  </si>
+  <si>
+    <t>Paul (3106583636) (D), Henry (6073399363), Adi (3103038889) (D)</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
     <t>Ezana (2405594003), Matheo (6462079196) (D)</t>
   </si>
   <si>
-    <t>Paul (3106583636) (D), Thor Waguespack (2404299065) (D), Edu (7862012521) (D)</t>
-  </si>
-  <si>
-    <t>Jack Mogelof (9172163044) (D)</t>
-  </si>
-  <si>
-    <t>Ben Kairouz (9179401653) (D), Kamsi (6465933923)</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
-    <t>Gabe Heller (7187220895) (D), Kamsi (6465933923)</t>
-  </si>
-  <si>
-    <t>Jaxon (4159881691) (D), Paul (3106583636) (D), Alejandro L (2676633214)</t>
-  </si>
-  <si>
-    <t>Jack Mogelof (9172163044) (D), Jamari Pitchford (7738297627) (D), Edu (7862012521) (D)</t>
-  </si>
-  <si>
-    <t>Ben Kairouz (9179401653) (D), Thor Waguespack (2404299065) (D), Alejandro E. Ulvert (3058421968) (D)</t>
-  </si>
-  <si>
-    <t>Ali Awada (6469771844), Blake Steel (6109995081) (D), Harry Corbin (5182223247) (D)</t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
-    <t>Gabe Heller (7187220895) (D), Harry Corbin (5182223247) (D)</t>
-  </si>
-  <si>
-    <t>Jaxon (4159881691) (D), Alejandro L (2676633214), Alejandro Espinosa (7866702380) (D)</t>
-  </si>
-  <si>
-    <t>Josh Greene (9176368454) (D), Ali Awada (6469771844), Alejandro E. Ulvert (3058421968) (D)</t>
-  </si>
-  <si>
-    <t>Ben Kairouz (9179401653) (D), Paul (3106583636) (D), George Ryckman (9176015863) (D)</t>
-  </si>
-  <si>
-    <t>Jamari Pitchford (7738297627) (D), Jake Dieterich (9177968225), Blake Steel (6109995081) (D)</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
-    <t>Josh Greene (9176368454) (D), George Ryckman (9176015863) (D)</t>
-  </si>
-  <si>
-    <t>Kamsi (6465933923), Alexander (9175433831) (D), Alejandro Espinosa (7866702380) (D)</t>
-  </si>
-  <si>
-    <t>Matheo (6462079196) (D), Edu (7862012521) (D), Ali Awada (6469771844)</t>
-  </si>
-  <si>
-    <t>Ben Kairouz (9179401653) (D), Henry (6073399363), Thor Waguespack (2404299065) (D)</t>
-  </si>
-  <si>
-    <t>Jamari Pitchford (7738297627) (D), Blake Steel (6109995081) (D), Noah Yaffe (6109995081) (D)</t>
-  </si>
-  <si>
-    <t>Ezana (2405594003), Alejandro E. Ulvert (3058421968) (D), Adi (3103038889) (D)</t>
+    <t>Jaxon (4159881691) (D), Ben Kairouz (9179401653) (D), Kamsi (6465933923)</t>
+  </si>
+  <si>
+    <t>Paul (3106583636) (D), Ali Awada (6469771844), Harry Corbin (5182223247) (D)</t>
+  </si>
+  <si>
+    <t>Jack Mogelof (9172163044) (D), Gabe Heller (7187220895) (D), Jake Dieterich (9177968225)</t>
+  </si>
+  <si>
+    <t>Alejandro L (2676633214), Alejandro Espinosa (7866702380) (D), Noah Yaffe (6109995081) (D)</t>
+  </si>
+  <si>
+    <t>Alexander (9175433831) (D), Josh Greene (9176368454) (D), Henry (6073399363)</t>
   </si>
 </sst>
 </file>

</xml_diff>